<commit_message>
Update Kho gửi phòng sxbh 12_2025.xlsx
</commit_message>
<xml_diff>
--- a/5. Other/Thiết bị kho gửi/2025/Kho gửi phòng sxbh 12_2025.xlsx
+++ b/5. Other/Thiết bị kho gửi/2025/Kho gửi phòng sxbh 12_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VNET\5. Other\Thiết bị kho gửi\2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9755AC-804E-475E-9370-556984D088FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D370202-FAE4-4E31-B2DF-F99212585EB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -609,18 +609,18 @@
       </c>
       <c r="E5" s="3">
         <f>Xuất!AH6+'Hủy tb'!AH6</f>
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="F5" s="3">
         <f t="shared" ref="F5:F6" si="0">C5+D5-E5</f>
-        <v>72</v>
+        <v>8</v>
       </c>
       <c r="G5" s="3">
         <v>0</v>
       </c>
       <c r="H5" s="3">
         <f t="shared" ref="H5" si="1">F5-G5</f>
-        <v>72</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1793,7 +1793,7 @@
   <dimension ref="A1:AH19"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="K23" sqref="K23:K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2032,7 +2032,9 @@
       <c r="B6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="6">
+        <v>64</v>
+      </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
@@ -2065,7 +2067,7 @@
       <c r="AG6" s="7"/>
       <c r="AH6" s="7">
         <f t="shared" ref="AH6:AH19" si="0">SUM(C6:AG6)</f>
-        <v>0</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">

</xml_diff>